<commit_message>
fix #50 ensure results equal + misc changes
add todo message near business income hardcoded rates
update results
add note in io docs for mort interest assumption
</commit_message>
<xml_diff>
--- a/current_io_docs.xlsx
+++ b/current_io_docs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Amir\Documents\git_repos\taxsim\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C1D9945-C020-4416-A91D-52DAD91133EB}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C45D9B6-85E3-4DB4-A092-828DE5925D97}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16185" windowHeight="7410" xr2:uid="{D03C11A7-0F7D-4097-B472-E5FA9DA97E82}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="74">
   <si>
     <t>filing_status</t>
   </si>
@@ -247,6 +247,12 @@
   </si>
   <si>
     <t>Taxable Income Calculation</t>
+  </si>
+  <si>
+    <t>MARG_RATE_BOUND</t>
+  </si>
+  <si>
+    <t>ASSUMED_MORTGAGE_RATE</t>
   </si>
 </sst>
 </file>
@@ -666,8 +672,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A248377F-C8B0-4405-98F3-3E7614809E38}">
   <dimension ref="E1:P31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -844,6 +850,12 @@
       <c r="E15" t="s">
         <v>12</v>
       </c>
+      <c r="F15" t="s">
+        <v>72</v>
+      </c>
+      <c r="G15" t="s">
+        <v>73</v>
+      </c>
       <c r="M15" s="1" t="s">
         <v>16</v>
       </c>

</xml_diff>

<commit_message>
update pipenv packages update gitignore add sched_se_tax to io docs
</commit_message>
<xml_diff>
--- a/current_io_docs.xlsx
+++ b/current_io_docs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10123"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Amir\Documents\git_repos\taxsim\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aelsi/Documents/taxsim/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F31AD0B7-DFA9-4D03-8F86-D5DF45DA3971}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{587B051A-19A9-B349-88DD-6EFA87C18F5E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16185" windowHeight="7410" xr2:uid="{D03C11A7-0F7D-4097-B472-E5FA9DA97E82}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="18860" xr2:uid="{D03C11A7-0F7D-4097-B472-E5FA9DA97E82}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,6 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -31,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="76">
   <si>
     <t>agi</t>
   </si>
@@ -253,6 +252,12 @@
   </si>
   <si>
     <t>Total income subject to tax after adjustments for exclusions and additions.</t>
+  </si>
+  <si>
+    <t>sched_se_tax</t>
+  </si>
+  <si>
+    <t>Self-Employment Tax</t>
   </si>
 </sst>
 </file>
@@ -809,29 +814,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A248377F-C8B0-4405-98F3-3E7614809E38}">
-  <dimension ref="A1:M36"/>
+  <dimension ref="A1:M37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="35.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="74.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="74.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="48" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="35.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="126.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.140625" customWidth="1"/>
-    <col min="12" max="12" width="33.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="65.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="34.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="35.28515625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="111.42578125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="126.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.1640625" customWidth="1"/>
+    <col min="12" max="12" width="33.83203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="65.83203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="34.1640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="35.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="111.5" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="29.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" ht="24" x14ac:dyDescent="0.3">
       <c r="A1" s="15" t="s">
         <v>63</v>
       </c>
@@ -848,7 +853,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="B2" s="14" t="s">
         <v>14</v>
       </c>
@@ -856,13 +861,13 @@
         <v>64</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B3" s="12"/>
       <c r="C3" s="12"/>
       <c r="D3" s="12"/>
       <c r="E3" s="12"/>
     </row>
-    <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="16" t="s">
         <v>53</v>
       </c>
@@ -877,7 +882,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="16"/>
       <c r="B5" s="8" t="s">
         <v>66</v>
@@ -888,7 +893,7 @@
       <c r="D5" s="6"/>
       <c r="E5" s="7"/>
     </row>
-    <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="16"/>
       <c r="B6" s="8" t="s">
         <v>0</v>
@@ -901,7 +906,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="16"/>
       <c r="B7" s="8" t="s">
         <v>1</v>
@@ -914,7 +919,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="16"/>
       <c r="B8" s="8" t="s">
         <v>13</v>
@@ -927,7 +932,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="16"/>
       <c r="B9" s="8" t="s">
         <v>69</v>
@@ -940,7 +945,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="16"/>
       <c r="B10" s="4" t="s">
         <v>14</v>
@@ -953,7 +958,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="16"/>
       <c r="B11" s="8" t="s">
         <v>68</v>
@@ -966,16 +971,16 @@
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B12" s="12"/>
       <c r="C12" s="12"/>
       <c r="D12" s="12"/>
       <c r="E12" s="12"/>
     </row>
-    <row r="13" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="12"/>
     </row>
-    <row r="14" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="17" t="s">
         <v>56</v>
       </c>
@@ -990,7 +995,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="17"/>
       <c r="B15" s="13" t="s">
         <v>2</v>
@@ -1000,7 +1005,7 @@
       </c>
       <c r="E15" s="1"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="17"/>
       <c r="B16" s="13" t="s">
         <v>3</v>
@@ -1012,7 +1017,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="17"/>
       <c r="B17" s="13" t="s">
         <v>5</v>
@@ -1022,7 +1027,7 @@
       </c>
       <c r="E17" s="1"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="17"/>
       <c r="B18" s="13" t="s">
         <v>4</v>
@@ -1032,7 +1037,7 @@
       </c>
       <c r="E18" s="1"/>
     </row>
-    <row r="19" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="17"/>
       <c r="B19" s="8" t="s">
         <v>1</v>
@@ -1043,7 +1048,7 @@
       <c r="D19" s="6"/>
       <c r="E19" s="7"/>
     </row>
-    <row r="20" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="B20" s="8" t="s">
         <v>46</v>
       </c>
@@ -1055,7 +1060,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="17" t="s">
         <v>54</v>
       </c>
@@ -1070,7 +1075,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="B24" s="8" t="s">
         <v>7</v>
       </c>
@@ -1082,7 +1087,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B25" s="8" t="s">
         <v>8</v>
       </c>
@@ -1091,7 +1096,7 @@
       </c>
       <c r="D25" s="6"/>
     </row>
-    <row r="28" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="17" t="s">
         <v>55</v>
       </c>
@@ -1106,7 +1111,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="17"/>
       <c r="B29" s="13" t="s">
         <v>47</v>
@@ -1118,7 +1123,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="17"/>
       <c r="B30" s="13" t="s">
         <v>10</v>
@@ -1128,7 +1133,7 @@
       </c>
       <c r="E30" s="3"/>
     </row>
-    <row r="31" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" s="17"/>
       <c r="B31" s="8" t="s">
         <v>49</v>
@@ -1139,7 +1144,7 @@
       <c r="D31" s="6"/>
       <c r="E31" s="7"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="17"/>
       <c r="B32" s="13" t="s">
         <v>12</v>
@@ -1151,7 +1156,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A33" s="17"/>
       <c r="B33" s="13" t="s">
         <v>11</v>
@@ -1163,36 +1168,46 @@
         <v>27</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A34" s="17"/>
       <c r="B34" s="13" t="s">
-        <v>48</v>
+        <v>74</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>52</v>
+        <v>75</v>
       </c>
       <c r="E34" s="3"/>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A35" s="17"/>
       <c r="B35" s="13" t="s">
-        <v>9</v>
+        <v>48</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>29</v>
+        <v>52</v>
       </c>
       <c r="E35" s="3"/>
       <c r="M35" s="12"/>
     </row>
-    <row r="36" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B36" s="8" t="s">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A36" s="17"/>
+      <c r="B36" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E36" s="3"/>
+    </row>
+    <row r="37" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="B37" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C36" s="5" t="s">
+      <c r="C37" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="D36" s="6"/>
-      <c r="E36" s="7"/>
+      <c r="D37" s="6"/>
+      <c r="E37" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>